<commit_message>
Ejecucion lista s,s varios escenarios
</commit_message>
<xml_diff>
--- a/src/s_s_pronosticos_escenarios.xlsx
+++ b/src/s_s_pronosticos_escenarios.xlsx
@@ -432,28 +432,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-5524348.360000003</v>
+        <v>-5569949.620000001</v>
       </c>
       <c r="C2">
-        <v>28313</v>
+        <v>28031</v>
       </c>
       <c r="D2">
-        <v>3475</v>
+        <v>3581</v>
       </c>
       <c r="E2">
-        <v>859</v>
+        <v>936</v>
       </c>
       <c r="F2">
-        <v>1593</v>
+        <v>1800</v>
       </c>
       <c r="G2">
-        <v>31960</v>
+        <v>31652</v>
       </c>
       <c r="H2">
-        <v>123069084</v>
+        <v>122111716</v>
       </c>
       <c r="I2">
-        <v>166245.9379373337</v>
+        <v>172629.7538743076</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -461,28 +461,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6778648.960000001</v>
+        <v>-14606866.04</v>
       </c>
       <c r="C3">
-        <v>28455</v>
+        <v>28227</v>
       </c>
       <c r="D3">
-        <v>3622</v>
+        <v>3465</v>
       </c>
       <c r="E3">
-        <v>772</v>
+        <v>809</v>
       </c>
       <c r="F3">
-        <v>1479</v>
+        <v>1506</v>
       </c>
       <c r="G3">
-        <v>32079</v>
+        <v>31962</v>
       </c>
       <c r="H3">
-        <v>118687471</v>
+        <v>132401544</v>
       </c>
       <c r="I3">
-        <v>168796.8218594036</v>
+        <v>165319.1821221222</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -490,28 +490,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-2601691.620000001</v>
+        <v>-6575933.620000001</v>
       </c>
       <c r="C4">
-        <v>28361</v>
+        <v>28195</v>
       </c>
       <c r="D4">
-        <v>3607</v>
+        <v>3562</v>
       </c>
       <c r="E4">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="F4">
-        <v>1484</v>
+        <v>1574</v>
       </c>
       <c r="G4">
-        <v>31962</v>
+        <v>32077</v>
       </c>
       <c r="H4">
-        <v>126726992</v>
+        <v>124335302</v>
       </c>
       <c r="I4">
-        <v>164619.2202944125</v>
+        <v>162720.2151138777</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -519,28 +519,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-4426719.200000003</v>
+        <v>-8571221.359999999</v>
       </c>
       <c r="C5">
-        <v>28458</v>
+        <v>28278</v>
       </c>
       <c r="D5">
-        <v>3619</v>
+        <v>3686</v>
       </c>
       <c r="E5">
-        <v>709</v>
+        <v>961</v>
       </c>
       <c r="F5">
-        <v>1368</v>
+        <v>1727</v>
       </c>
       <c r="G5">
-        <v>32419</v>
+        <v>31720</v>
       </c>
       <c r="H5">
-        <v>122091668</v>
+        <v>127652872</v>
       </c>
       <c r="I5">
-        <v>165794.3990297768</v>
+        <v>178962.956460973</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -548,28 +548,28 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6516721.380000003</v>
+        <v>14699896.8</v>
       </c>
       <c r="C6">
-        <v>28094</v>
+        <v>28331</v>
       </c>
       <c r="D6">
-        <v>3659</v>
+        <v>3513</v>
       </c>
       <c r="E6">
-        <v>917</v>
+        <v>891</v>
       </c>
       <c r="F6">
-        <v>1645</v>
+        <v>1584</v>
       </c>
       <c r="G6">
-        <v>31685</v>
+        <v>32153</v>
       </c>
       <c r="H6">
-        <v>115146568</v>
+        <v>112095396</v>
       </c>
       <c r="I6">
-        <v>176446.9722190281</v>
+        <v>166608.9059479931</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -577,28 +577,28 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-14883548.04</v>
+        <v>12323558.22</v>
       </c>
       <c r="C7">
-        <v>28331</v>
+        <v>28361</v>
       </c>
       <c r="D7">
-        <v>3808</v>
+        <v>3752</v>
       </c>
       <c r="E7">
-        <v>927</v>
+        <v>812</v>
       </c>
       <c r="F7">
-        <v>1679</v>
+        <v>1581</v>
       </c>
       <c r="G7">
-        <v>32091</v>
+        <v>31914</v>
       </c>
       <c r="H7">
-        <v>130575723</v>
+        <v>112096172</v>
       </c>
       <c r="I7">
-        <v>171389.5054624535</v>
+        <v>174994.4412646393</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -606,28 +606,28 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-20183979.94000001</v>
+        <v>-7702800.039999999</v>
       </c>
       <c r="C8">
-        <v>28251</v>
+        <v>28128</v>
       </c>
       <c r="D8">
-        <v>3619</v>
+        <v>3706</v>
       </c>
       <c r="E8">
-        <v>881</v>
+        <v>949</v>
       </c>
       <c r="F8">
-        <v>1672</v>
+        <v>1721</v>
       </c>
       <c r="G8">
-        <v>32051</v>
+        <v>31795</v>
       </c>
       <c r="H8">
-        <v>133681209</v>
+        <v>124016222</v>
       </c>
       <c r="I8">
-        <v>163710.5284009175</v>
+        <v>172112.4384295688</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -635,28 +635,28 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-2883632.619999997</v>
+        <v>8605763.639999997</v>
       </c>
       <c r="C9">
-        <v>28415</v>
+        <v>28461</v>
       </c>
       <c r="D9">
-        <v>3653</v>
+        <v>3777</v>
       </c>
       <c r="E9">
-        <v>890</v>
+        <v>717</v>
       </c>
       <c r="F9">
-        <v>1631</v>
+        <v>1308</v>
       </c>
       <c r="G9">
-        <v>32149</v>
+        <v>32114</v>
       </c>
       <c r="H9">
-        <v>125262488</v>
+        <v>118680371</v>
       </c>
       <c r="I9">
-        <v>168827.9635108062</v>
+        <v>177576.0175825561</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -664,28 +664,28 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3345813.959999997</v>
+        <v>-5056496.620000005</v>
       </c>
       <c r="C10">
-        <v>28392</v>
+        <v>28322</v>
       </c>
       <c r="D10">
-        <v>3597</v>
+        <v>3550</v>
       </c>
       <c r="E10">
-        <v>853</v>
+        <v>931</v>
       </c>
       <c r="F10">
-        <v>1509</v>
+        <v>1676</v>
       </c>
       <c r="G10">
-        <v>32006</v>
+        <v>32113</v>
       </c>
       <c r="H10">
-        <v>121412839</v>
+        <v>123540786</v>
       </c>
       <c r="I10">
-        <v>168623.8492133844</v>
+        <v>164482.1975427587</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -693,28 +693,28 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-12103341.88</v>
+        <v>-7761189.039999999</v>
       </c>
       <c r="C11">
-        <v>28451</v>
+        <v>28184</v>
       </c>
       <c r="D11">
-        <v>3566</v>
+        <v>3601</v>
       </c>
       <c r="E11">
-        <v>840</v>
+        <v>826</v>
       </c>
       <c r="F11">
-        <v>1547</v>
+        <v>1587</v>
       </c>
       <c r="G11">
-        <v>32030</v>
+        <v>31921</v>
       </c>
       <c r="H11">
-        <v>129404580</v>
+        <v>125786246</v>
       </c>
       <c r="I11">
-        <v>175921.826895424</v>
+        <v>165521.2679124412</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -722,28 +722,28 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-24227966.36</v>
+        <v>-15908105.04</v>
       </c>
       <c r="C12">
-        <v>28022</v>
+        <v>28224</v>
       </c>
       <c r="D12">
-        <v>3506</v>
+        <v>3573</v>
       </c>
       <c r="E12">
-        <v>885</v>
+        <v>808</v>
       </c>
       <c r="F12">
-        <v>1544</v>
+        <v>1491</v>
       </c>
       <c r="G12">
-        <v>31886</v>
+        <v>32062</v>
       </c>
       <c r="H12">
-        <v>134769956</v>
+        <v>132925001</v>
       </c>
       <c r="I12">
-        <v>162216.0137760983</v>
+        <v>161083.2516938325</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -751,28 +751,28 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>7282426.640000001</v>
+        <v>1986505.799999997</v>
       </c>
       <c r="C13">
-        <v>28281</v>
+        <v>28202</v>
       </c>
       <c r="D13">
-        <v>3764</v>
+        <v>3587</v>
       </c>
       <c r="E13">
-        <v>759</v>
+        <v>907</v>
       </c>
       <c r="F13">
-        <v>1532</v>
+        <v>1581</v>
       </c>
       <c r="G13">
-        <v>31928</v>
+        <v>31898</v>
       </c>
       <c r="H13">
-        <v>114600336</v>
+        <v>121104781</v>
       </c>
       <c r="I13">
-        <v>175976.5960035097</v>
+        <v>168993.5181644078</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -780,28 +780,28 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-12533164.94</v>
+        <v>-3875995.039999999</v>
       </c>
       <c r="C14">
-        <v>28335</v>
+        <v>28448</v>
       </c>
       <c r="D14">
-        <v>3605</v>
+        <v>3581</v>
       </c>
       <c r="E14">
-        <v>855</v>
+        <v>830</v>
       </c>
       <c r="F14">
-        <v>1554</v>
+        <v>1521</v>
       </c>
       <c r="G14">
-        <v>32194</v>
+        <v>32142</v>
       </c>
       <c r="H14">
-        <v>130429267</v>
+        <v>124855386</v>
       </c>
       <c r="I14">
-        <v>164488.5454048989</v>
+        <v>172612.8803203162</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -809,28 +809,28 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>10802609.64</v>
+        <v>-10073422.45999999</v>
       </c>
       <c r="C15">
-        <v>28192</v>
+        <v>28017</v>
       </c>
       <c r="D15">
-        <v>3642</v>
+        <v>3843</v>
       </c>
       <c r="E15">
-        <v>889</v>
+        <v>950</v>
       </c>
       <c r="F15">
-        <v>1619</v>
+        <v>1660</v>
       </c>
       <c r="G15">
-        <v>31972</v>
+        <v>31650</v>
       </c>
       <c r="H15">
-        <v>115528068</v>
+        <v>127193158</v>
       </c>
       <c r="I15">
-        <v>167405.6956515671</v>
+        <v>167787.3752995825</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -838,28 +838,28 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-6357494.359999999</v>
+        <v>-2849854.200000003</v>
       </c>
       <c r="C16">
-        <v>28232</v>
+        <v>28276</v>
       </c>
       <c r="D16">
-        <v>3594</v>
+        <v>3846</v>
       </c>
       <c r="E16">
-        <v>908</v>
+        <v>855</v>
       </c>
       <c r="F16">
-        <v>1643</v>
+        <v>1431</v>
       </c>
       <c r="G16">
-        <v>31938</v>
+        <v>32029</v>
       </c>
       <c r="H16">
-        <v>124376658</v>
+        <v>122562844</v>
       </c>
       <c r="I16">
-        <v>172352.044573715</v>
+        <v>166678.4827930715</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -867,28 +867,28 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-12473545.62</v>
+        <v>-20915235.62</v>
       </c>
       <c r="C17">
-        <v>28029</v>
+        <v>28241</v>
       </c>
       <c r="D17">
-        <v>3673</v>
+        <v>3671</v>
       </c>
       <c r="E17">
-        <v>912</v>
+        <v>948</v>
       </c>
       <c r="F17">
-        <v>1638</v>
+        <v>1753</v>
       </c>
       <c r="G17">
-        <v>31785</v>
+        <v>31991</v>
       </c>
       <c r="H17">
-        <v>128496925</v>
+        <v>131448170</v>
       </c>
       <c r="I17">
-        <v>169503.7057528853</v>
+        <v>170641.3562135771</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -896,28 +896,28 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2001031.120000001</v>
+        <v>1498288.379999997</v>
       </c>
       <c r="C18">
-        <v>28021</v>
+        <v>28335</v>
       </c>
       <c r="D18">
-        <v>3707</v>
+        <v>3732</v>
       </c>
       <c r="E18">
-        <v>932</v>
+        <v>871</v>
       </c>
       <c r="F18">
-        <v>1689</v>
+        <v>1541</v>
       </c>
       <c r="G18">
-        <v>31574</v>
+        <v>32082</v>
       </c>
       <c r="H18">
-        <v>117343268</v>
+        <v>122943712</v>
       </c>
       <c r="I18">
-        <v>170738.198851674</v>
+        <v>167662.402093123</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -925,28 +925,28 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-8196743.199999999</v>
+        <v>-3911230.940000001</v>
       </c>
       <c r="C19">
-        <v>28174</v>
+        <v>28098</v>
       </c>
       <c r="D19">
-        <v>3712</v>
+        <v>3765</v>
       </c>
       <c r="E19">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="F19">
-        <v>1497</v>
+        <v>1565</v>
       </c>
       <c r="G19">
-        <v>31951</v>
+        <v>31757</v>
       </c>
       <c r="H19">
-        <v>125178219</v>
+        <v>120211860</v>
       </c>
       <c r="I19">
-        <v>167443.6639021537</v>
+        <v>171582.7190423718</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -954,28 +954,28 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-5468744.459999997</v>
+        <v>-12094988.04</v>
       </c>
       <c r="C20">
-        <v>28337</v>
+        <v>28172</v>
       </c>
       <c r="D20">
-        <v>3424</v>
+        <v>3675</v>
       </c>
       <c r="E20">
-        <v>819</v>
+        <v>862</v>
       </c>
       <c r="F20">
-        <v>1621</v>
+        <v>1729</v>
       </c>
       <c r="G20">
-        <v>32060</v>
+        <v>31896</v>
       </c>
       <c r="H20">
-        <v>126953850</v>
+        <v>126178760</v>
       </c>
       <c r="I20">
-        <v>162130.1832320454</v>
+        <v>168136.9091094931</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -983,28 +983,28 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-12299914.04</v>
+        <v>7265001.799999997</v>
       </c>
       <c r="C21">
-        <v>28563</v>
+        <v>28378</v>
       </c>
       <c r="D21">
-        <v>3711</v>
+        <v>3758</v>
       </c>
       <c r="E21">
-        <v>767</v>
+        <v>822</v>
       </c>
       <c r="F21">
-        <v>1324</v>
+        <v>1482</v>
       </c>
       <c r="G21">
-        <v>32494</v>
+        <v>31971</v>
       </c>
       <c r="H21">
-        <v>132532105</v>
+        <v>118339180</v>
       </c>
       <c r="I21">
-        <v>168712.6147012332</v>
+        <v>174054.4744758561</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1012,28 +1012,28 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-9597351.040000007</v>
+        <v>-6160070.619999997</v>
       </c>
       <c r="C22">
-        <v>28294</v>
+        <v>28067</v>
       </c>
       <c r="D22">
-        <v>3987</v>
+        <v>3550</v>
       </c>
       <c r="E22">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="F22">
-        <v>1741</v>
+        <v>1747</v>
       </c>
       <c r="G22">
-        <v>31872</v>
+        <v>31639</v>
       </c>
       <c r="H22">
-        <v>125722747</v>
+        <v>125365219</v>
       </c>
       <c r="I22">
-        <v>176296.9601174032</v>
+        <v>168453.5923502101</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1041,28 +1041,28 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-2598866.619999997</v>
+        <v>13756931.64</v>
       </c>
       <c r="C23">
-        <v>28567</v>
+        <v>28172</v>
       </c>
       <c r="D23">
-        <v>3638</v>
+        <v>3759</v>
       </c>
       <c r="E23">
-        <v>919</v>
+        <v>904</v>
       </c>
       <c r="F23">
-        <v>1650</v>
+        <v>1612</v>
       </c>
       <c r="G23">
-        <v>32201</v>
+        <v>31618</v>
       </c>
       <c r="H23">
-        <v>122437357</v>
+        <v>111264122</v>
       </c>
       <c r="I23">
-        <v>180499.7671128158</v>
+        <v>178236.6950457849</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1070,28 +1070,28 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-10124757.36</v>
+        <v>4532429.800000001</v>
       </c>
       <c r="C24">
-        <v>28174</v>
+        <v>28109</v>
       </c>
       <c r="D24">
-        <v>3594</v>
+        <v>3602</v>
       </c>
       <c r="E24">
-        <v>865</v>
+        <v>844</v>
       </c>
       <c r="F24">
-        <v>1557</v>
+        <v>1631</v>
       </c>
       <c r="G24">
-        <v>31944</v>
+        <v>31667</v>
       </c>
       <c r="H24">
-        <v>127502181</v>
+        <v>119085559</v>
       </c>
       <c r="I24">
-        <v>163645.2487045712</v>
+        <v>173144.8148301715</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1099,28 +1099,28 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-17943722.72</v>
+        <v>8542060.960000001</v>
       </c>
       <c r="C25">
-        <v>28277</v>
+        <v>28239</v>
       </c>
       <c r="D25">
-        <v>3496</v>
+        <v>3658</v>
       </c>
       <c r="E25">
-        <v>865</v>
+        <v>882</v>
       </c>
       <c r="F25">
-        <v>1569</v>
+        <v>1696</v>
       </c>
       <c r="G25">
-        <v>32048</v>
+        <v>31937</v>
       </c>
       <c r="H25">
-        <v>135237359</v>
+        <v>113576164</v>
       </c>
       <c r="I25">
-        <v>157986.6403397994</v>
+        <v>170100.830071821</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1128,28 +1128,28 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-1171991.52</v>
+        <v>10967882.96</v>
       </c>
       <c r="C26">
-        <v>28334</v>
+        <v>28353</v>
       </c>
       <c r="D26">
-        <v>3705</v>
+        <v>3651</v>
       </c>
       <c r="E26">
-        <v>842</v>
+        <v>818</v>
       </c>
       <c r="F26">
-        <v>1480</v>
+        <v>1455</v>
       </c>
       <c r="G26">
-        <v>31960</v>
+        <v>31958</v>
       </c>
       <c r="H26">
-        <v>122098126</v>
+        <v>116664660</v>
       </c>
       <c r="I26">
-        <v>176125.9249030782</v>
+        <v>172226.3823127814</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1157,28 +1157,28 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-17474751.62</v>
+        <v>-9672751.039999999</v>
       </c>
       <c r="C27">
-        <v>28344</v>
+        <v>28337</v>
       </c>
       <c r="D27">
-        <v>3609</v>
+        <v>3493</v>
       </c>
       <c r="E27">
-        <v>864</v>
+        <v>813</v>
       </c>
       <c r="F27">
-        <v>1602</v>
+        <v>1544</v>
       </c>
       <c r="G27">
-        <v>32084</v>
+        <v>31999</v>
       </c>
       <c r="H27">
-        <v>132551648</v>
+        <v>127961286</v>
       </c>
       <c r="I27">
-        <v>170309.8969537524</v>
+        <v>171643.2501281083</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1186,28 +1186,28 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-3865585.879999999</v>
+        <v>1801553.799999997</v>
       </c>
       <c r="C28">
-        <v>28467</v>
+        <v>28018</v>
       </c>
       <c r="D28">
-        <v>3620</v>
+        <v>3896</v>
       </c>
       <c r="E28">
-        <v>769</v>
+        <v>1000</v>
       </c>
       <c r="F28">
-        <v>1538</v>
+        <v>1761</v>
       </c>
       <c r="G28">
-        <v>32330</v>
+        <v>31641</v>
       </c>
       <c r="H28">
-        <v>122463047</v>
+        <v>116053231</v>
       </c>
       <c r="I28">
-        <v>163236.1876520574</v>
+        <v>174226.0510365062</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1215,28 +1215,28 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1832118.219999999</v>
+        <v>-10910746.62</v>
       </c>
       <c r="C29">
-        <v>28045</v>
+        <v>28175</v>
       </c>
       <c r="D29">
-        <v>3842</v>
+        <v>3540</v>
       </c>
       <c r="E29">
-        <v>1032</v>
+        <v>825</v>
       </c>
       <c r="F29">
-        <v>1798</v>
+        <v>1575</v>
       </c>
       <c r="G29">
-        <v>31761</v>
+        <v>31811</v>
       </c>
       <c r="H29">
-        <v>117310078</v>
+        <v>127180971</v>
       </c>
       <c r="I29">
-        <v>171253.5493269355</v>
+        <v>170862.0792102675</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1244,28 +1244,28 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-5973517.52</v>
+        <v>1715826.959999997</v>
       </c>
       <c r="C30">
-        <v>28175</v>
+        <v>28375</v>
       </c>
       <c r="D30">
-        <v>3803</v>
+        <v>3772</v>
       </c>
       <c r="E30">
-        <v>843</v>
+        <v>881</v>
       </c>
       <c r="F30">
-        <v>1578</v>
+        <v>1657</v>
       </c>
       <c r="G30">
-        <v>31813</v>
+        <v>32096</v>
       </c>
       <c r="H30">
-        <v>127098497</v>
+        <v>120072253</v>
       </c>
       <c r="I30">
-        <v>171909.7341590075</v>
+        <v>168163.8303559448</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1273,28 +1273,28 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>2163810.219999999</v>
+        <v>14689742.8</v>
       </c>
       <c r="C31">
-        <v>28417</v>
+        <v>28357</v>
       </c>
       <c r="D31">
-        <v>3422</v>
+        <v>3595</v>
       </c>
       <c r="E31">
-        <v>777</v>
+        <v>876</v>
       </c>
       <c r="F31">
-        <v>1425</v>
+        <v>1574</v>
       </c>
       <c r="G31">
-        <v>32098</v>
+        <v>31781</v>
       </c>
       <c r="H31">
-        <v>123119364</v>
+        <v>113345186</v>
       </c>
       <c r="I31">
-        <v>163897.9612892817</v>
+        <v>175438.5827677562</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1302,28 +1302,28 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-1796700.360000003</v>
+        <v>-9459520.619999997</v>
       </c>
       <c r="C32">
-        <v>28260</v>
+        <v>28044</v>
       </c>
       <c r="D32">
-        <v>3692</v>
+        <v>3567</v>
       </c>
       <c r="E32">
-        <v>849</v>
+        <v>864</v>
       </c>
       <c r="F32">
-        <v>1514</v>
+        <v>1642</v>
       </c>
       <c r="G32">
-        <v>31995</v>
+        <v>31615</v>
       </c>
       <c r="H32">
-        <v>122757840</v>
+        <v>125631524</v>
       </c>
       <c r="I32">
-        <v>169007.3085211352</v>
+        <v>170253.7254052114</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1331,28 +1331,28 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-6454791.620000005</v>
+        <v>966015.9600000009</v>
       </c>
       <c r="C33">
-        <v>28277</v>
+        <v>28244</v>
       </c>
       <c r="D33">
-        <v>3568</v>
+        <v>3512</v>
       </c>
       <c r="E33">
-        <v>789</v>
+        <v>897</v>
       </c>
       <c r="F33">
-        <v>1447</v>
+        <v>1552</v>
       </c>
       <c r="G33">
-        <v>32111</v>
+        <v>31921</v>
       </c>
       <c r="H33">
-        <v>126380615</v>
+        <v>120615861</v>
       </c>
       <c r="I33">
-        <v>164550.3901320223</v>
+        <v>167184.2000014486</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1360,28 +1360,28 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>14067668.12</v>
+        <v>-14050998.04</v>
       </c>
       <c r="C34">
-        <v>28521</v>
+        <v>28147</v>
       </c>
       <c r="D34">
-        <v>3685</v>
+        <v>3498</v>
       </c>
       <c r="E34">
-        <v>758</v>
+        <v>789</v>
       </c>
       <c r="F34">
-        <v>1432</v>
+        <v>1476</v>
       </c>
       <c r="G34">
-        <v>32205</v>
+        <v>31828</v>
       </c>
       <c r="H34">
-        <v>115640205</v>
+        <v>129365585</v>
       </c>
       <c r="I34">
-        <v>173595.5419781806</v>
+        <v>170318.361711319</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1389,28 +1389,28 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>731088.5399999991</v>
+        <v>-1333844.620000001</v>
       </c>
       <c r="C35">
-        <v>28459</v>
+        <v>28041</v>
       </c>
       <c r="D35">
-        <v>3738</v>
+        <v>3537</v>
       </c>
       <c r="E35">
-        <v>822</v>
+        <v>887</v>
       </c>
       <c r="F35">
-        <v>1448</v>
+        <v>1609</v>
       </c>
       <c r="G35">
-        <v>32084</v>
+        <v>31721</v>
       </c>
       <c r="H35">
-        <v>122897580</v>
+        <v>121648725</v>
       </c>
       <c r="I35">
-        <v>170038.0502148318</v>
+        <v>171773.6543172656</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1418,28 +1418,28 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>13113477.38</v>
+        <v>-807153.3600000031</v>
       </c>
       <c r="C36">
-        <v>28229</v>
+        <v>28409</v>
       </c>
       <c r="D36">
-        <v>3772</v>
+        <v>3658</v>
       </c>
       <c r="E36">
-        <v>899</v>
+        <v>834</v>
       </c>
       <c r="F36">
-        <v>1640</v>
+        <v>1549</v>
       </c>
       <c r="G36">
-        <v>31791</v>
+        <v>32078</v>
       </c>
       <c r="H36">
-        <v>111063971</v>
+        <v>121453152</v>
       </c>
       <c r="I36">
-        <v>174655.6833926138</v>
+        <v>169545.5224690815</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1447,28 +1447,28 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>-18442749.88</v>
+        <v>433204.6400000006</v>
       </c>
       <c r="C37">
-        <v>28302</v>
+        <v>28031</v>
       </c>
       <c r="D37">
-        <v>3486</v>
+        <v>3611</v>
       </c>
       <c r="E37">
-        <v>889</v>
+        <v>909</v>
       </c>
       <c r="F37">
-        <v>1631</v>
+        <v>1614</v>
       </c>
       <c r="G37">
-        <v>31834</v>
+        <v>31636</v>
       </c>
       <c r="H37">
-        <v>134472597</v>
+        <v>119501404</v>
       </c>
       <c r="I37">
-        <v>174668.6109688711</v>
+        <v>170279.5745352979</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1476,28 +1476,28 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>-7410448.199999999</v>
+        <v>1832385.379999999</v>
       </c>
       <c r="C38">
-        <v>28326</v>
+        <v>28075</v>
       </c>
       <c r="D38">
-        <v>3675</v>
+        <v>3745</v>
       </c>
       <c r="E38">
-        <v>778</v>
+        <v>1019</v>
       </c>
       <c r="F38">
-        <v>1514</v>
+        <v>1890</v>
       </c>
       <c r="G38">
-        <v>31987</v>
+        <v>31724</v>
       </c>
       <c r="H38">
-        <v>127136398</v>
+        <v>115257033</v>
       </c>
       <c r="I38">
-        <v>168637.6677351622</v>
+        <v>174505.4230287572</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1505,28 +1505,28 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>-11440324.46</v>
+        <v>-2768505.940000001</v>
       </c>
       <c r="C39">
-        <v>28156</v>
+        <v>28420</v>
       </c>
       <c r="D39">
-        <v>3582</v>
+        <v>3684</v>
       </c>
       <c r="E39">
-        <v>911</v>
+        <v>809</v>
       </c>
       <c r="F39">
-        <v>1693</v>
+        <v>1491</v>
       </c>
       <c r="G39">
-        <v>31827</v>
+        <v>32214</v>
       </c>
       <c r="H39">
-        <v>130652955</v>
+        <v>122524490</v>
       </c>
       <c r="I39">
-        <v>167458.2731203178</v>
+        <v>165742.2936729187</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1534,28 +1534,28 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>5833984.799999999</v>
+        <v>-13295802.3</v>
       </c>
       <c r="C40">
-        <v>28317</v>
+        <v>28286</v>
       </c>
       <c r="D40">
-        <v>3753</v>
+        <v>3645</v>
       </c>
       <c r="E40">
-        <v>781</v>
+        <v>768</v>
       </c>
       <c r="F40">
-        <v>1437</v>
+        <v>1537</v>
       </c>
       <c r="G40">
-        <v>31899</v>
+        <v>32068</v>
       </c>
       <c r="H40">
-        <v>116446041</v>
+        <v>128865288</v>
       </c>
       <c r="I40">
-        <v>173844.1900905131</v>
+        <v>166439.6780877738</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1563,28 +1563,28 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>5384419.539999999</v>
+        <v>-9425883.039999999</v>
       </c>
       <c r="C41">
-        <v>28187</v>
+        <v>28305</v>
       </c>
       <c r="D41">
-        <v>3630</v>
+        <v>3861</v>
       </c>
       <c r="E41">
-        <v>853</v>
+        <v>793</v>
       </c>
       <c r="F41">
-        <v>1598</v>
+        <v>1503</v>
       </c>
       <c r="G41">
-        <v>31760</v>
+        <v>32155</v>
       </c>
       <c r="H41">
-        <v>118045212</v>
+        <v>126258655</v>
       </c>
       <c r="I41">
-        <v>172866.4565035829</v>
+        <v>170825.5967175688</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1592,28 +1592,28 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1474630.380000003</v>
+        <v>-12132085.2</v>
       </c>
       <c r="C42">
-        <v>28481</v>
+        <v>28252</v>
       </c>
       <c r="D42">
-        <v>3879</v>
+        <v>3580</v>
       </c>
       <c r="E42">
-        <v>831</v>
+        <v>909</v>
       </c>
       <c r="F42">
-        <v>1586</v>
+        <v>1592</v>
       </c>
       <c r="G42">
-        <v>32160</v>
+        <v>32048</v>
       </c>
       <c r="H42">
-        <v>121897358</v>
+        <v>128705325</v>
       </c>
       <c r="I42">
-        <v>177997.5787050549</v>
+        <v>169765.7398274234</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1621,28 +1621,28 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-8719886.459999997</v>
+        <v>-8945574.620000001</v>
       </c>
       <c r="C43">
-        <v>28505</v>
+        <v>28191</v>
       </c>
       <c r="D43">
-        <v>3458</v>
+        <v>3757</v>
       </c>
       <c r="E43">
-        <v>775</v>
+        <v>860</v>
       </c>
       <c r="F43">
-        <v>1402</v>
+        <v>1539</v>
       </c>
       <c r="G43">
-        <v>32276</v>
+        <v>31806</v>
       </c>
       <c r="H43">
-        <v>130004800</v>
+        <v>128754763</v>
       </c>
       <c r="I43">
-        <v>164802.9703801712</v>
+        <v>168926.50989728</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1650,28 +1650,28 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-20016343.2</v>
+        <v>-990006.1999999993</v>
       </c>
       <c r="C44">
-        <v>28310</v>
+        <v>28314</v>
       </c>
       <c r="D44">
-        <v>3490</v>
+        <v>3655</v>
       </c>
       <c r="E44">
-        <v>949</v>
+        <v>922</v>
       </c>
       <c r="F44">
-        <v>1716</v>
+        <v>1595</v>
       </c>
       <c r="G44">
-        <v>32152</v>
+        <v>32030</v>
       </c>
       <c r="H44">
-        <v>136629296</v>
+        <v>121307621</v>
       </c>
       <c r="I44">
-        <v>160157.1709946475</v>
+        <v>168500.8720621371</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1679,28 +1679,28 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>-3699016.359999999</v>
+        <v>1232338.640000001</v>
       </c>
       <c r="C45">
-        <v>28510</v>
+        <v>28373</v>
       </c>
       <c r="D45">
-        <v>3510</v>
+        <v>3680</v>
       </c>
       <c r="E45">
-        <v>772</v>
+        <v>849</v>
       </c>
       <c r="F45">
-        <v>1506</v>
+        <v>1614</v>
       </c>
       <c r="G45">
-        <v>32201</v>
+        <v>31825</v>
       </c>
       <c r="H45">
-        <v>125165320</v>
+        <v>119523936</v>
       </c>
       <c r="I45">
-        <v>169308.2428670913</v>
+        <v>180438.6339665847</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1708,28 +1708,28 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>2555765.379999995</v>
+        <v>-2772184.620000005</v>
       </c>
       <c r="C46">
-        <v>28409</v>
+        <v>28089</v>
       </c>
       <c r="D46">
-        <v>3646</v>
+        <v>3629</v>
       </c>
       <c r="E46">
-        <v>844</v>
+        <v>945</v>
       </c>
       <c r="F46">
-        <v>1540</v>
+        <v>1650</v>
       </c>
       <c r="G46">
-        <v>32161</v>
+        <v>31704</v>
       </c>
       <c r="H46">
-        <v>119820318</v>
+        <v>124903254</v>
       </c>
       <c r="I46">
-        <v>168651.6454242262</v>
+        <v>167346.0238363855</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1737,28 +1737,28 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>-9132841.200000003</v>
+        <v>-13326957.46</v>
       </c>
       <c r="C47">
-        <v>28276</v>
+        <v>28122</v>
       </c>
       <c r="D47">
-        <v>3684</v>
+        <v>3619</v>
       </c>
       <c r="E47">
-        <v>803</v>
+        <v>856</v>
       </c>
       <c r="F47">
-        <v>1462</v>
+        <v>1468</v>
       </c>
       <c r="G47">
-        <v>31960</v>
+        <v>31968</v>
       </c>
       <c r="H47">
-        <v>127263756</v>
+        <v>129076373</v>
       </c>
       <c r="I47">
-        <v>174748.9314835552</v>
+        <v>162413.754972665</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1766,28 +1766,28 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>4139872.220000001</v>
+        <v>-8556001.460000001</v>
       </c>
       <c r="C48">
-        <v>28347</v>
+        <v>28302</v>
       </c>
       <c r="D48">
-        <v>3744</v>
+        <v>3739</v>
       </c>
       <c r="E48">
-        <v>819</v>
+        <v>954</v>
       </c>
       <c r="F48">
-        <v>1512</v>
+        <v>1683</v>
       </c>
       <c r="G48">
-        <v>32000</v>
+        <v>32066</v>
       </c>
       <c r="H48">
-        <v>121647593</v>
+        <v>124092693</v>
       </c>
       <c r="I48">
-        <v>174338.1522881514</v>
+        <v>172866.082972993</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1795,28 +1795,28 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>6384938.799999997</v>
+        <v>-1333362.039999999</v>
       </c>
       <c r="C49">
-        <v>28102</v>
+        <v>28426</v>
       </c>
       <c r="D49">
-        <v>3615</v>
+        <v>3732</v>
       </c>
       <c r="E49">
-        <v>936</v>
+        <v>785</v>
       </c>
       <c r="F49">
-        <v>1613</v>
+        <v>1427</v>
       </c>
       <c r="G49">
-        <v>31583</v>
+        <v>32180</v>
       </c>
       <c r="H49">
-        <v>118774302</v>
+        <v>123370367</v>
       </c>
       <c r="I49">
-        <v>172785.7831778519</v>
+        <v>166251.615758685</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1824,28 +1824,28 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>-6659390.199999999</v>
+        <v>1725457.799999997</v>
       </c>
       <c r="C50">
-        <v>28481</v>
+        <v>28389</v>
       </c>
       <c r="D50">
-        <v>3736</v>
+        <v>3651</v>
       </c>
       <c r="E50">
-        <v>840</v>
+        <v>826</v>
       </c>
       <c r="F50">
-        <v>1525</v>
+        <v>1527</v>
       </c>
       <c r="G50">
-        <v>32264</v>
+        <v>32084</v>
       </c>
       <c r="H50">
-        <v>126902515</v>
+        <v>120680285</v>
       </c>
       <c r="I50">
-        <v>167463.0202667676</v>
+        <v>168866.2770287305</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1853,28 +1853,28 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>-5559778.040000003</v>
+        <v>6323202.219999999</v>
       </c>
       <c r="C51">
-        <v>28565</v>
+        <v>28349</v>
       </c>
       <c r="D51">
-        <v>3499</v>
+        <v>3906</v>
       </c>
       <c r="E51">
-        <v>879</v>
+        <v>951</v>
       </c>
       <c r="F51">
-        <v>1628</v>
+        <v>1759</v>
       </c>
       <c r="G51">
-        <v>32308</v>
+        <v>31868</v>
       </c>
       <c r="H51">
-        <v>124109932</v>
+        <v>114683940</v>
       </c>
       <c r="I51">
-        <v>168405.7933660351</v>
+        <v>183847.8058786305</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1882,28 +1882,28 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>-11143468.04</v>
+        <v>2768766.539999999</v>
       </c>
       <c r="C52">
-        <v>28183</v>
+        <v>28204</v>
       </c>
       <c r="D52">
-        <v>3953</v>
+        <v>3801</v>
       </c>
       <c r="E52">
-        <v>876</v>
+        <v>891</v>
       </c>
       <c r="F52">
-        <v>1601</v>
+        <v>1533</v>
       </c>
       <c r="G52">
-        <v>31874</v>
+        <v>31745</v>
       </c>
       <c r="H52">
-        <v>128531332</v>
+        <v>120862466</v>
       </c>
       <c r="I52">
-        <v>169348.0521381369</v>
+        <v>177366.7568828567</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1911,28 +1911,28 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>3825738.280000001</v>
+        <v>-6087406.200000003</v>
       </c>
       <c r="C53">
-        <v>28324</v>
+        <v>28474</v>
       </c>
       <c r="D53">
-        <v>3455</v>
+        <v>3641</v>
       </c>
       <c r="E53">
-        <v>813</v>
+        <v>822</v>
       </c>
       <c r="F53">
-        <v>1471</v>
+        <v>1482</v>
       </c>
       <c r="G53">
-        <v>31925</v>
+        <v>32188</v>
       </c>
       <c r="H53">
-        <v>121657390</v>
+        <v>126574709</v>
       </c>
       <c r="I53">
-        <v>173425.1099103812</v>
+        <v>170402.8728982047</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1940,28 +1940,28 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>-15086215.46</v>
+        <v>5728412.539999999</v>
       </c>
       <c r="C54">
-        <v>28347</v>
+        <v>28442</v>
       </c>
       <c r="D54">
-        <v>3876</v>
+        <v>3942</v>
       </c>
       <c r="E54">
-        <v>868</v>
+        <v>851</v>
       </c>
       <c r="F54">
-        <v>1534</v>
+        <v>1562</v>
       </c>
       <c r="G54">
-        <v>32128</v>
+        <v>32250</v>
       </c>
       <c r="H54">
-        <v>131702910</v>
+        <v>117357486</v>
       </c>
       <c r="I54">
-        <v>164675.4787844148</v>
+        <v>173319.2508275418</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1969,28 +1969,28 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>295268.9600000009</v>
+        <v>-9015748.459999997</v>
       </c>
       <c r="C55">
-        <v>28262</v>
+        <v>28337</v>
       </c>
       <c r="D55">
-        <v>3658</v>
+        <v>3349</v>
       </c>
       <c r="E55">
-        <v>846</v>
+        <v>835</v>
       </c>
       <c r="F55">
-        <v>1524</v>
+        <v>1499</v>
       </c>
       <c r="G55">
-        <v>31835</v>
+        <v>32177</v>
       </c>
       <c r="H55">
-        <v>120286442</v>
+        <v>128173071</v>
       </c>
       <c r="I55">
-        <v>175859.242190456</v>
+        <v>163702.6834534416</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1998,28 +1998,28 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>-4555560.939999998</v>
+        <v>-8766961.780000001</v>
       </c>
       <c r="C56">
-        <v>28316</v>
+        <v>28275</v>
       </c>
       <c r="D56">
-        <v>3694</v>
+        <v>3681</v>
       </c>
       <c r="E56">
-        <v>828</v>
+        <v>848</v>
       </c>
       <c r="F56">
-        <v>1529</v>
+        <v>1548</v>
       </c>
       <c r="G56">
-        <v>32011</v>
+        <v>31961</v>
       </c>
       <c r="H56">
-        <v>126678414</v>
+        <v>128793316</v>
       </c>
       <c r="I56">
-        <v>171427.533883573</v>
+        <v>166933.5639251817</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2027,28 +2027,28 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>8872932.960000001</v>
+        <v>-9172317.780000001</v>
       </c>
       <c r="C57">
-        <v>28524</v>
+        <v>28236</v>
       </c>
       <c r="D57">
-        <v>3560</v>
+        <v>3629</v>
       </c>
       <c r="E57">
-        <v>739</v>
+        <v>984</v>
       </c>
       <c r="F57">
-        <v>1381</v>
+        <v>1706</v>
       </c>
       <c r="G57">
-        <v>32198</v>
+        <v>31797</v>
       </c>
       <c r="H57">
-        <v>118142168</v>
+        <v>124087667</v>
       </c>
       <c r="I57">
-        <v>174076.9473269025</v>
+        <v>178180.9021472683</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2056,28 +2056,28 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>5028629.439999998</v>
+        <v>-5054127.200000003</v>
       </c>
       <c r="C58">
-        <v>28238</v>
+        <v>28323</v>
       </c>
       <c r="D58">
-        <v>3611</v>
+        <v>3672</v>
       </c>
       <c r="E58">
-        <v>787</v>
+        <v>929</v>
       </c>
       <c r="F58">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="G58">
-        <v>31953</v>
+        <v>32141</v>
       </c>
       <c r="H58">
-        <v>116823742</v>
+        <v>121312201</v>
       </c>
       <c r="I58">
-        <v>167929.8792036022</v>
+        <v>169231.8938207554</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2085,28 +2085,28 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>-5485809.940000001</v>
+        <v>-9214558.200000003</v>
       </c>
       <c r="C59">
-        <v>28367</v>
+        <v>28298</v>
       </c>
       <c r="D59">
-        <v>3685</v>
+        <v>3499</v>
       </c>
       <c r="E59">
-        <v>765</v>
+        <v>790</v>
       </c>
       <c r="F59">
-        <v>1488</v>
+        <v>1506</v>
       </c>
       <c r="G59">
-        <v>32054</v>
+        <v>32069</v>
       </c>
       <c r="H59">
-        <v>122609034</v>
+        <v>128059929</v>
       </c>
       <c r="I59">
-        <v>174540.705212118</v>
+        <v>163249.447366691</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2114,28 +2114,28 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>3126501.479999997</v>
+        <v>392566.5399999991</v>
       </c>
       <c r="C60">
-        <v>28469</v>
+        <v>28269</v>
       </c>
       <c r="D60">
-        <v>3471</v>
+        <v>3530</v>
       </c>
       <c r="E60">
-        <v>885</v>
+        <v>843</v>
       </c>
       <c r="F60">
-        <v>1526</v>
+        <v>1542</v>
       </c>
       <c r="G60">
-        <v>32245</v>
+        <v>31867</v>
       </c>
       <c r="H60">
-        <v>120312446</v>
+        <v>124407165</v>
       </c>
       <c r="I60">
-        <v>164943.0719226018</v>
+        <v>176705.5852582638</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2143,28 +2143,28 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>1906780.479999997</v>
+        <v>19637.79999999702</v>
       </c>
       <c r="C61">
-        <v>28143</v>
+        <v>28137</v>
       </c>
       <c r="D61">
-        <v>3842</v>
+        <v>3650</v>
       </c>
       <c r="E61">
-        <v>960</v>
+        <v>856</v>
       </c>
       <c r="F61">
-        <v>1760</v>
+        <v>1508</v>
       </c>
       <c r="G61">
-        <v>31831</v>
+        <v>31900</v>
       </c>
       <c r="H61">
-        <v>118854042</v>
+        <v>119513103</v>
       </c>
       <c r="I61">
-        <v>174103.1164002033</v>
+        <v>164947.3738408832</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2172,28 +2172,28 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>-9801751.359999999</v>
+        <v>3853557.539999999</v>
       </c>
       <c r="C62">
-        <v>28599</v>
+        <v>28163</v>
       </c>
       <c r="D62">
-        <v>3600</v>
+        <v>3584</v>
       </c>
       <c r="E62">
-        <v>794</v>
+        <v>823</v>
       </c>
       <c r="F62">
-        <v>1528</v>
+        <v>1566</v>
       </c>
       <c r="G62">
-        <v>32534</v>
+        <v>31759</v>
       </c>
       <c r="H62">
-        <v>127873637</v>
+        <v>118961212</v>
       </c>
       <c r="I62">
-        <v>165946.6234675394</v>
+        <v>169535.4819180947</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2201,28 +2201,28 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>-4028780.460000001</v>
+        <v>-17843230.88</v>
       </c>
       <c r="C63">
-        <v>28265</v>
+        <v>28006</v>
       </c>
       <c r="D63">
-        <v>3875</v>
+        <v>3559</v>
       </c>
       <c r="E63">
         <v>919</v>
       </c>
       <c r="F63">
-        <v>1654</v>
+        <v>1575</v>
       </c>
       <c r="G63">
-        <v>31910</v>
+        <v>31748</v>
       </c>
       <c r="H63">
-        <v>123037168</v>
+        <v>132184850</v>
       </c>
       <c r="I63">
-        <v>170997.2703659226</v>
+        <v>164535.2593997813</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2230,28 +2230,28 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>3744971.219999999</v>
+        <v>-5292843.779999997</v>
       </c>
       <c r="C64">
-        <v>28363</v>
+        <v>28441</v>
       </c>
       <c r="D64">
-        <v>3688</v>
+        <v>3517</v>
       </c>
       <c r="E64">
-        <v>864</v>
+        <v>819</v>
       </c>
       <c r="F64">
-        <v>1587</v>
+        <v>1582</v>
       </c>
       <c r="G64">
-        <v>32169</v>
+        <v>32272</v>
       </c>
       <c r="H64">
-        <v>117584516</v>
+        <v>125000672</v>
       </c>
       <c r="I64">
-        <v>169488.4741346792</v>
+        <v>163780.8597455487</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2259,28 +2259,28 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>-745986.299999997</v>
+        <v>-18125375.88</v>
       </c>
       <c r="C65">
-        <v>27924</v>
+        <v>28419</v>
       </c>
       <c r="D65">
-        <v>3564</v>
+        <v>3528</v>
       </c>
       <c r="E65">
-        <v>927</v>
+        <v>798</v>
       </c>
       <c r="F65">
-        <v>1784</v>
+        <v>1498</v>
       </c>
       <c r="G65">
-        <v>31398</v>
+        <v>32248</v>
       </c>
       <c r="H65">
-        <v>118061700</v>
+        <v>134620277</v>
       </c>
       <c r="I65">
-        <v>176497.5287869758</v>
+        <v>162499.8570745482</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2288,28 +2288,28 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>-8919829.359999999</v>
+        <v>-3325193.200000003</v>
       </c>
       <c r="C66">
-        <v>28313</v>
+        <v>28132</v>
       </c>
       <c r="D66">
-        <v>3610</v>
+        <v>3630</v>
       </c>
       <c r="E66">
-        <v>801</v>
+        <v>837</v>
       </c>
       <c r="F66">
-        <v>1491</v>
+        <v>1524</v>
       </c>
       <c r="G66">
-        <v>32061</v>
+        <v>31761</v>
       </c>
       <c r="H66">
-        <v>125710436</v>
+        <v>124617183</v>
       </c>
       <c r="I66">
-        <v>166814.7193585607</v>
+        <v>167752.2838901663</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2317,28 +2317,28 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-8984174.359999999</v>
+        <v>-12086952.62</v>
       </c>
       <c r="C67">
-        <v>28448</v>
+        <v>28084</v>
       </c>
       <c r="D67">
-        <v>3679</v>
+        <v>3689</v>
       </c>
       <c r="E67">
-        <v>792</v>
+        <v>945</v>
       </c>
       <c r="F67">
-        <v>1454</v>
+        <v>1643</v>
       </c>
       <c r="G67">
-        <v>32286</v>
+        <v>31979</v>
       </c>
       <c r="H67">
-        <v>126435958</v>
+        <v>126103989</v>
       </c>
       <c r="I67">
-        <v>168202.540068686</v>
+        <v>160896.1753854641</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2346,28 +2346,28 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>3725165.699999999</v>
+        <v>2779804.539999999</v>
       </c>
       <c r="C68">
-        <v>28301</v>
+        <v>28306</v>
       </c>
       <c r="D68">
-        <v>3718</v>
+        <v>3594</v>
       </c>
       <c r="E68">
-        <v>869</v>
+        <v>829</v>
       </c>
       <c r="F68">
-        <v>1588</v>
+        <v>1481</v>
       </c>
       <c r="G68">
-        <v>31800</v>
+        <v>32103</v>
       </c>
       <c r="H68">
-        <v>120838552</v>
+        <v>119114076</v>
       </c>
       <c r="I68">
-        <v>178487.6354685731</v>
+        <v>164301.8434315165</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2375,28 +2375,28 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>-11171915.94</v>
+        <v>-13681486.52</v>
       </c>
       <c r="C69">
-        <v>28308</v>
+        <v>28376</v>
       </c>
       <c r="D69">
-        <v>3566</v>
+        <v>3505</v>
       </c>
       <c r="E69">
-        <v>827</v>
+        <v>877</v>
       </c>
       <c r="F69">
-        <v>1474</v>
+        <v>1615</v>
       </c>
       <c r="G69">
-        <v>32182</v>
+        <v>32079</v>
       </c>
       <c r="H69">
-        <v>128928641</v>
+        <v>128135000</v>
       </c>
       <c r="I69">
-        <v>164836.6825923741</v>
+        <v>169812.9837444696</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2404,28 +2404,28 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>7649930.219999999</v>
+        <v>-7111230.360000003</v>
       </c>
       <c r="C70">
-        <v>28290</v>
+        <v>28370</v>
       </c>
       <c r="D70">
-        <v>3469</v>
+        <v>3691</v>
       </c>
       <c r="E70">
-        <v>883</v>
+        <v>741</v>
       </c>
       <c r="F70">
-        <v>1561</v>
+        <v>1379</v>
       </c>
       <c r="G70">
-        <v>31855</v>
+        <v>32076</v>
       </c>
       <c r="H70">
-        <v>116344407</v>
+        <v>127947725</v>
       </c>
       <c r="I70">
-        <v>169768.9575234514</v>
+        <v>172180.5349428579</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2433,28 +2433,28 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>-11199695.88</v>
+        <v>5700191.379999997</v>
       </c>
       <c r="C71">
-        <v>28480</v>
+        <v>28339</v>
       </c>
       <c r="D71">
-        <v>3692</v>
+        <v>3660</v>
       </c>
       <c r="E71">
-        <v>804</v>
+        <v>818</v>
       </c>
       <c r="F71">
-        <v>1430</v>
+        <v>1452</v>
       </c>
       <c r="G71">
-        <v>32276</v>
+        <v>31991</v>
       </c>
       <c r="H71">
-        <v>127710397</v>
+        <v>118040539</v>
       </c>
       <c r="I71">
-        <v>171933.7040734134</v>
+        <v>169767.4492968111</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2462,28 +2462,28 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>10327446.38</v>
+        <v>-5874981.619999997</v>
       </c>
       <c r="C72">
-        <v>28347</v>
+        <v>28182</v>
       </c>
       <c r="D72">
-        <v>3687</v>
+        <v>3541</v>
       </c>
       <c r="E72">
-        <v>814</v>
+        <v>975</v>
       </c>
       <c r="F72">
-        <v>1483</v>
+        <v>1716</v>
       </c>
       <c r="G72">
-        <v>31971</v>
+        <v>31862</v>
       </c>
       <c r="H72">
-        <v>116612918</v>
+        <v>123029245</v>
       </c>
       <c r="I72">
-        <v>169742.8661195344</v>
+        <v>172656.2527661844</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2491,28 +2491,28 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>-3714986.779999997</v>
+        <v>-2239709.199999999</v>
       </c>
       <c r="C73">
-        <v>28328</v>
+        <v>28315</v>
       </c>
       <c r="D73">
-        <v>3603</v>
+        <v>3768</v>
       </c>
       <c r="E73">
-        <v>826</v>
+        <v>858</v>
       </c>
       <c r="F73">
-        <v>1541</v>
+        <v>1522</v>
       </c>
       <c r="G73">
-        <v>31916</v>
+        <v>31892</v>
       </c>
       <c r="H73">
-        <v>121657681</v>
+        <v>123366212</v>
       </c>
       <c r="I73">
-        <v>176450.9400153471</v>
+        <v>175687.0995118613</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2520,28 +2520,28 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>2658939.800000001</v>
+        <v>-10885912.62</v>
       </c>
       <c r="C74">
-        <v>28436</v>
+        <v>28378</v>
       </c>
       <c r="D74">
-        <v>3549</v>
+        <v>3726</v>
       </c>
       <c r="E74">
-        <v>819</v>
+        <v>890</v>
       </c>
       <c r="F74">
-        <v>1533</v>
+        <v>1679</v>
       </c>
       <c r="G74">
-        <v>32076</v>
+        <v>32128</v>
       </c>
       <c r="H74">
-        <v>121708203</v>
+        <v>127999609</v>
       </c>
       <c r="I74">
-        <v>172792.3592989953</v>
+        <v>171326.1950811262</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -2549,28 +2549,28 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>-428185.4599999972</v>
+        <v>-3979104.460000001</v>
       </c>
       <c r="C75">
-        <v>27981</v>
+        <v>28228</v>
       </c>
       <c r="D75">
-        <v>3643</v>
+        <v>3803</v>
       </c>
       <c r="E75">
-        <v>1020</v>
+        <v>817</v>
       </c>
       <c r="F75">
-        <v>1729</v>
+        <v>1564</v>
       </c>
       <c r="G75">
-        <v>31574</v>
+        <v>31836</v>
       </c>
       <c r="H75">
-        <v>121288934</v>
+        <v>122742959</v>
       </c>
       <c r="I75">
-        <v>166925.7125870456</v>
+        <v>179475.4488446525</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -2578,28 +2578,28 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>5259397.379999999</v>
+        <v>-3409372.780000001</v>
       </c>
       <c r="C76">
-        <v>28443</v>
+        <v>28244</v>
       </c>
       <c r="D76">
-        <v>3596</v>
+        <v>3677</v>
       </c>
       <c r="E76">
-        <v>866</v>
+        <v>979</v>
       </c>
       <c r="F76">
-        <v>1514</v>
+        <v>1826</v>
       </c>
       <c r="G76">
-        <v>32129</v>
+        <v>31888</v>
       </c>
       <c r="H76">
-        <v>118826553</v>
+        <v>121303814</v>
       </c>
       <c r="I76">
-        <v>173700.4075115214</v>
+        <v>177731.1151882253</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2607,28 +2607,28 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>-17268889.2</v>
+        <v>2983043.540000003</v>
       </c>
       <c r="C77">
-        <v>27812</v>
+        <v>28146</v>
       </c>
       <c r="D77">
-        <v>3691</v>
+        <v>3940</v>
       </c>
       <c r="E77">
-        <v>971</v>
+        <v>934</v>
       </c>
       <c r="F77">
-        <v>1951</v>
+        <v>1641</v>
       </c>
       <c r="G77">
-        <v>31427</v>
+        <v>31856</v>
       </c>
       <c r="H77">
-        <v>125292045</v>
+        <v>113761383</v>
       </c>
       <c r="I77">
-        <v>170916.5804628821</v>
+        <v>174630.1656866862</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2636,28 +2636,28 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>-20631967.94</v>
+        <v>-19202025.36</v>
       </c>
       <c r="C78">
-        <v>28332</v>
+        <v>28301</v>
       </c>
       <c r="D78">
-        <v>3569</v>
+        <v>3648</v>
       </c>
       <c r="E78">
-        <v>868</v>
+        <v>846</v>
       </c>
       <c r="F78">
-        <v>1541</v>
+        <v>1550</v>
       </c>
       <c r="G78">
-        <v>32123</v>
+        <v>32089</v>
       </c>
       <c r="H78">
-        <v>133294444</v>
+        <v>131299688</v>
       </c>
       <c r="I78">
-        <v>167323.4677614721</v>
+        <v>169127.34223154</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2665,28 +2665,28 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>6591209.960000001</v>
+        <v>-14583617.14</v>
       </c>
       <c r="C79">
-        <v>27988</v>
+        <v>28269</v>
       </c>
       <c r="D79">
-        <v>3487</v>
+        <v>3649</v>
       </c>
       <c r="E79">
-        <v>901</v>
+        <v>810</v>
       </c>
       <c r="F79">
-        <v>1713</v>
+        <v>1479</v>
       </c>
       <c r="G79">
-        <v>31611</v>
+        <v>32193</v>
       </c>
       <c r="H79">
-        <v>114609110</v>
+        <v>131502360</v>
       </c>
       <c r="I79">
-        <v>167360.7228858134</v>
+        <v>167287.1104755459</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -2694,28 +2694,28 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>-31840266.77999999</v>
+        <v>-11356136.2</v>
       </c>
       <c r="C80">
-        <v>28080</v>
+        <v>28298</v>
       </c>
       <c r="D80">
-        <v>3411</v>
+        <v>3800</v>
       </c>
       <c r="E80">
-        <v>873</v>
+        <v>842</v>
       </c>
       <c r="F80">
-        <v>1813</v>
+        <v>1590</v>
       </c>
       <c r="G80">
-        <v>32069</v>
+        <v>32044</v>
       </c>
       <c r="H80">
-        <v>137357900</v>
+        <v>124916613</v>
       </c>
       <c r="I80">
-        <v>160014.7656121368</v>
+        <v>170963.2799240178</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -2723,28 +2723,28 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>-28519085.04</v>
+        <v>-3493510.619999997</v>
       </c>
       <c r="C81">
-        <v>28516</v>
+        <v>28257</v>
       </c>
       <c r="D81">
-        <v>3778</v>
+        <v>3565</v>
       </c>
       <c r="E81">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="F81">
-        <v>1387</v>
+        <v>1450</v>
       </c>
       <c r="G81">
-        <v>32420</v>
+        <v>32046</v>
       </c>
       <c r="H81">
-        <v>143848589</v>
+        <v>121663969</v>
       </c>
       <c r="I81">
-        <v>162054.8846793196</v>
+        <v>165158.7945374964</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -2752,28 +2752,28 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>861664.4400000013</v>
+        <v>-7378757.620000001</v>
       </c>
       <c r="C82">
-        <v>28021</v>
+        <v>28212</v>
       </c>
       <c r="D82">
-        <v>3465</v>
+        <v>3611</v>
       </c>
       <c r="E82">
-        <v>933</v>
+        <v>821</v>
       </c>
       <c r="F82">
-        <v>1753</v>
+        <v>1492</v>
       </c>
       <c r="G82">
-        <v>31522</v>
+        <v>31858</v>
       </c>
       <c r="H82">
-        <v>117607488</v>
+        <v>125545167</v>
       </c>
       <c r="I82">
-        <v>172525.3945572826</v>
+        <v>174362.172193437</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -2781,28 +2781,28 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>-1167759.460000001</v>
+        <v>-13612118.62</v>
       </c>
       <c r="C83">
-        <v>28334</v>
+        <v>28193</v>
       </c>
       <c r="D83">
-        <v>3748</v>
+        <v>3574</v>
       </c>
       <c r="E83">
-        <v>853</v>
+        <v>888</v>
       </c>
       <c r="F83">
-        <v>1561</v>
+        <v>1601</v>
       </c>
       <c r="G83">
-        <v>32077</v>
+        <v>31935</v>
       </c>
       <c r="H83">
-        <v>121118500</v>
+        <v>130087680</v>
       </c>
       <c r="I83">
-        <v>167666.7046805213</v>
+        <v>163472.9063190803</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -2810,28 +2810,28 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>-17870622.04</v>
+        <v>-22685555.62</v>
       </c>
       <c r="C84">
-        <v>28157</v>
+        <v>28326</v>
       </c>
       <c r="D84">
-        <v>3604</v>
+        <v>3590</v>
       </c>
       <c r="E84">
-        <v>773</v>
+        <v>778</v>
       </c>
       <c r="F84">
-        <v>1586</v>
+        <v>1508</v>
       </c>
       <c r="G84">
-        <v>31775</v>
+        <v>32106</v>
       </c>
       <c r="H84">
-        <v>130981700</v>
+        <v>138376361</v>
       </c>
       <c r="I84">
-        <v>173153.3178518176</v>
+        <v>163942.692109816</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -2839,28 +2839,28 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>-10496106.36</v>
+        <v>-7875763.039999999</v>
       </c>
       <c r="C85">
-        <v>28209</v>
+        <v>28452</v>
       </c>
       <c r="D85">
-        <v>3792</v>
+        <v>3449</v>
       </c>
       <c r="E85">
-        <v>958</v>
+        <v>813</v>
       </c>
       <c r="F85">
-        <v>1733</v>
+        <v>1443</v>
       </c>
       <c r="G85">
-        <v>31962</v>
+        <v>32198</v>
       </c>
       <c r="H85">
-        <v>125501926</v>
+        <v>129322247</v>
       </c>
       <c r="I85">
-        <v>170788.5342017563</v>
+        <v>171099.8791115417</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -2868,28 +2868,28 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>-4696025.300000001</v>
+        <v>-3450615.460000001</v>
       </c>
       <c r="C86">
-        <v>28211</v>
+        <v>28330</v>
       </c>
       <c r="D86">
-        <v>3490</v>
+        <v>3663</v>
       </c>
       <c r="E86">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="F86">
-        <v>1597</v>
+        <v>1506</v>
       </c>
       <c r="G86">
-        <v>31959</v>
+        <v>32125</v>
       </c>
       <c r="H86">
-        <v>125955520</v>
+        <v>124249315</v>
       </c>
       <c r="I86">
-        <v>165284.6021676726</v>
+        <v>170706.2957719533</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -2897,28 +2897,28 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>-3193856.939999998</v>
+        <v>-10219742.62</v>
       </c>
       <c r="C87">
-        <v>27991</v>
+        <v>28265</v>
       </c>
       <c r="D87">
-        <v>3616</v>
+        <v>3576</v>
       </c>
       <c r="E87">
-        <v>931</v>
+        <v>847</v>
       </c>
       <c r="F87">
-        <v>1748</v>
+        <v>1507</v>
       </c>
       <c r="G87">
-        <v>31536</v>
+        <v>32042</v>
       </c>
       <c r="H87">
-        <v>119963975</v>
+        <v>128984013</v>
       </c>
       <c r="I87">
-        <v>171696.440041646</v>
+        <v>164861.5399452213</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -2926,28 +2926,28 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>-19391880.62</v>
+        <v>-7721952.359999999</v>
       </c>
       <c r="C88">
-        <v>28414</v>
+        <v>28510</v>
       </c>
       <c r="D88">
-        <v>3658</v>
+        <v>3562</v>
       </c>
       <c r="E88">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="F88">
-        <v>1471</v>
+        <v>1475</v>
       </c>
       <c r="G88">
-        <v>32141</v>
+        <v>32357</v>
       </c>
       <c r="H88">
-        <v>134187470</v>
+        <v>128337174</v>
       </c>
       <c r="I88">
-        <v>173566.9182349858</v>
+        <v>167980.1654542289</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -2955,28 +2955,28 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>-1131068.359999999</v>
+        <v>-8937839.880000003</v>
       </c>
       <c r="C89">
-        <v>28472</v>
+        <v>28273</v>
       </c>
       <c r="D89">
-        <v>3542</v>
+        <v>3682</v>
       </c>
       <c r="E89">
-        <v>862</v>
+        <v>969</v>
       </c>
       <c r="F89">
-        <v>1498</v>
+        <v>1732</v>
       </c>
       <c r="G89">
-        <v>32119</v>
+        <v>31789</v>
       </c>
       <c r="H89">
-        <v>124913011</v>
+        <v>125721908</v>
       </c>
       <c r="I89">
-        <v>167717.2930286772</v>
+        <v>178886.2708346973</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -2984,28 +2984,28 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>2187509.380000001</v>
+        <v>-2339583.459999997</v>
       </c>
       <c r="C90">
-        <v>28152</v>
+        <v>28228</v>
       </c>
       <c r="D90">
-        <v>3588</v>
+        <v>3511</v>
       </c>
       <c r="E90">
-        <v>835</v>
+        <v>885</v>
       </c>
       <c r="F90">
-        <v>1488</v>
+        <v>1540</v>
       </c>
       <c r="G90">
-        <v>31765</v>
+        <v>32002</v>
       </c>
       <c r="H90">
-        <v>122066780</v>
+        <v>120182138</v>
       </c>
       <c r="I90">
-        <v>171315.5084703165</v>
+        <v>164276.754212453</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3013,28 +3013,28 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>9180472.799999997</v>
+        <v>-16316856.04</v>
       </c>
       <c r="C91">
-        <v>28538</v>
+        <v>28367</v>
       </c>
       <c r="D91">
-        <v>3779</v>
+        <v>3702</v>
       </c>
       <c r="E91">
-        <v>836</v>
+        <v>751</v>
       </c>
       <c r="F91">
-        <v>1527</v>
+        <v>1442</v>
       </c>
       <c r="G91">
-        <v>32213</v>
+        <v>32069</v>
       </c>
       <c r="H91">
-        <v>114275769</v>
+        <v>131579864</v>
       </c>
       <c r="I91">
-        <v>178331.6806972328</v>
+        <v>169232.3814593432</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3042,28 +3042,28 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>-12055890.2</v>
+        <v>11278247.12</v>
       </c>
       <c r="C92">
-        <v>28279</v>
+        <v>28292</v>
       </c>
       <c r="D92">
-        <v>3436</v>
+        <v>3644</v>
       </c>
       <c r="E92">
-        <v>863</v>
+        <v>825</v>
       </c>
       <c r="F92">
-        <v>1650</v>
+        <v>1560</v>
       </c>
       <c r="G92">
-        <v>31890</v>
+        <v>31931</v>
       </c>
       <c r="H92">
-        <v>130567211</v>
+        <v>112442569</v>
       </c>
       <c r="I92">
-        <v>168317.7565205278</v>
+        <v>171140.2803825201</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3071,28 +3071,28 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>-12492137.62</v>
+        <v>-7706503.200000003</v>
       </c>
       <c r="C93">
-        <v>28018</v>
+        <v>28101</v>
       </c>
       <c r="D93">
-        <v>3605</v>
+        <v>3551</v>
       </c>
       <c r="E93">
-        <v>960</v>
+        <v>779</v>
       </c>
       <c r="F93">
-        <v>1784</v>
+        <v>1462</v>
       </c>
       <c r="G93">
-        <v>31729</v>
+        <v>31868</v>
       </c>
       <c r="H93">
-        <v>127202859</v>
+        <v>124489834</v>
       </c>
       <c r="I93">
-        <v>165731.080190674</v>
+        <v>165654.4310274733</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3100,28 +3100,28 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>12122969.54</v>
+        <v>-5899995.780000001</v>
       </c>
       <c r="C94">
-        <v>28494</v>
+        <v>28347</v>
       </c>
       <c r="D94">
-        <v>3674</v>
+        <v>3751</v>
       </c>
       <c r="E94">
-        <v>778</v>
+        <v>838</v>
       </c>
       <c r="F94">
-        <v>1519</v>
+        <v>1480</v>
       </c>
       <c r="G94">
-        <v>32149</v>
+        <v>32025</v>
       </c>
       <c r="H94">
-        <v>111980979</v>
+        <v>122264854</v>
       </c>
       <c r="I94">
-        <v>175683.3622036512</v>
+        <v>173678.3664275819</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3129,28 +3129,28 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>2958252.800000001</v>
+        <v>-12536094.78</v>
       </c>
       <c r="C95">
-        <v>28418</v>
+        <v>28472</v>
       </c>
       <c r="D95">
-        <v>3695</v>
+        <v>3643</v>
       </c>
       <c r="E95">
-        <v>780</v>
+        <v>864</v>
       </c>
       <c r="F95">
-        <v>1478</v>
+        <v>1532</v>
       </c>
       <c r="G95">
-        <v>31972</v>
+        <v>32201</v>
       </c>
       <c r="H95">
-        <v>121623368</v>
+        <v>129055766</v>
       </c>
       <c r="I95">
-        <v>175210.8022465647</v>
+        <v>172053.4070199142</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3158,28 +3158,28 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>872862.9600000009</v>
+        <v>-2788412.780000001</v>
       </c>
       <c r="C96">
-        <v>28380</v>
+        <v>28499</v>
       </c>
       <c r="D96">
-        <v>3625</v>
+        <v>3685</v>
       </c>
       <c r="E96">
-        <v>805</v>
+        <v>829</v>
       </c>
       <c r="F96">
-        <v>1534</v>
+        <v>1507</v>
       </c>
       <c r="G96">
-        <v>32090</v>
+        <v>32195</v>
       </c>
       <c r="H96">
-        <v>118974310</v>
+        <v>124084537</v>
       </c>
       <c r="I96">
-        <v>176221.6887339161</v>
+        <v>171683.2286772138</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3187,28 +3187,28 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>-2473793.200000003</v>
+        <v>11983155.8</v>
       </c>
       <c r="C97">
-        <v>28189</v>
+        <v>28217</v>
       </c>
       <c r="D97">
-        <v>3731</v>
+        <v>3596</v>
       </c>
       <c r="E97">
-        <v>791</v>
+        <v>945</v>
       </c>
       <c r="F97">
-        <v>1464</v>
+        <v>1637</v>
       </c>
       <c r="G97">
-        <v>31878</v>
+        <v>31778</v>
       </c>
       <c r="H97">
-        <v>123593892</v>
+        <v>112195242</v>
       </c>
       <c r="I97">
-        <v>172808.2885961618</v>
+        <v>174004.4073201702</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3216,28 +3216,28 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>-14528919.36</v>
+        <v>-126198.4600000009</v>
       </c>
       <c r="C98">
-        <v>28196</v>
+        <v>28315</v>
       </c>
       <c r="D98">
-        <v>3643</v>
+        <v>3413</v>
       </c>
       <c r="E98">
-        <v>848</v>
+        <v>774</v>
       </c>
       <c r="F98">
-        <v>1543</v>
+        <v>1359</v>
       </c>
       <c r="G98">
-        <v>31980</v>
+        <v>31974</v>
       </c>
       <c r="H98">
-        <v>132263754</v>
+        <v>125768343</v>
       </c>
       <c r="I98">
-        <v>164791.3898348247</v>
+        <v>167337.3900552526</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3245,28 +3245,28 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>-9515201.780000001</v>
+        <v>13804869.22</v>
       </c>
       <c r="C99">
-        <v>28222</v>
+        <v>28074</v>
       </c>
       <c r="D99">
-        <v>3726</v>
+        <v>3847</v>
       </c>
       <c r="E99">
-        <v>880</v>
+        <v>802</v>
       </c>
       <c r="F99">
-        <v>1524</v>
+        <v>1561</v>
       </c>
       <c r="G99">
-        <v>31962</v>
+        <v>31651</v>
       </c>
       <c r="H99">
-        <v>126774338</v>
+        <v>112124176</v>
       </c>
       <c r="I99">
-        <v>167135.5301890327</v>
+        <v>172389.3496500508</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3274,28 +3274,28 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>-3381698.039999999</v>
+        <v>-2699497.459999997</v>
       </c>
       <c r="C100">
-        <v>28383</v>
+        <v>28057</v>
       </c>
       <c r="D100">
-        <v>3735</v>
+        <v>3671</v>
       </c>
       <c r="E100">
-        <v>796</v>
+        <v>923</v>
       </c>
       <c r="F100">
-        <v>1462</v>
+        <v>1710</v>
       </c>
       <c r="G100">
-        <v>32053</v>
+        <v>31662</v>
       </c>
       <c r="H100">
-        <v>126610990</v>
+        <v>120438875</v>
       </c>
       <c r="I100">
-        <v>172215.5582772332</v>
+        <v>170055.9293895279</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3303,28 +3303,28 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>-4429883.460000001</v>
+        <v>1620099.639999997</v>
       </c>
       <c r="C101">
-        <v>28457</v>
+        <v>28235</v>
       </c>
       <c r="D101">
-        <v>3625</v>
+        <v>3347</v>
       </c>
       <c r="E101">
-        <v>911</v>
+        <v>831</v>
       </c>
       <c r="F101">
-        <v>1588</v>
+        <v>1497</v>
       </c>
       <c r="G101">
-        <v>32036</v>
+        <v>31800</v>
       </c>
       <c r="H101">
-        <v>125000214</v>
+        <v>123247879</v>
       </c>
       <c r="I101">
-        <v>175913.8010960633</v>
+        <v>169653.9358841048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>